<commit_message>
Update Sample.xlsx add row
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yamaz\Documents\GitHub\github-actions-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39F451BF-58DA-457E-A72C-7B5EED06CF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56650601-E46F-4D1D-BDDD-5D7667C65573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38445" yWindow="3555" windowWidth="19275" windowHeight="17145" xr2:uid="{8541EB68-6030-448A-AA9E-D5F9FFCDD24D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
   <si>
     <t>col1</t>
     <phoneticPr fontId="1"/>
@@ -60,6 +60,16 @@
   <si>
     <t>item3</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>new_item1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>new_item2</t>
+  </si>
+  <si>
+    <t>new_item3</t>
   </si>
 </sst>
 </file>
@@ -461,13 +471,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15A0C46-738F-42E8-9DB4-F5B8BC35CF6F}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
@@ -588,6 +601,17 @@
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>